<commit_message>
more data cleaning and script updating
</commit_message>
<xml_diff>
--- a/data/lake-ontario/lake-ontario-spawning.xlsx
+++ b/data/lake-ontario/lake-ontario-spawning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-DegreeDay-Modeling/data/lake-ontario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB1788C-CACB-FE4C-8384-42BD2AF8D0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD02FC2-34FB-8C4C-80B0-9F3DA590A910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="500" windowWidth="17680" windowHeight="19220" xr2:uid="{88D49699-253E-9343-94D7-003220367E12}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="17680" windowHeight="19220" xr2:uid="{88D49699-253E-9343-94D7-003220367E12}"/>
   </bookViews>
   <sheets>
     <sheet name="lake-ontario-spawning" sheetId="1" r:id="rId1"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,14 +468,14 @@
         <v>39027</v>
       </c>
       <c r="B2" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:C13" si="0">MONTH(A2)</f>
+        <f>MONTH(A2)</f>
         <v>11</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D13" si="1">DAY(A2)</f>
+        <f>DAY(A2)</f>
         <v>6</v>
       </c>
       <c r="E2">
@@ -500,14 +500,14 @@
         <v>39028</v>
       </c>
       <c r="B3" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A3)</f>
         <v>11</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" si="1"/>
+        <f>DAY(A3)</f>
         <v>7</v>
       </c>
       <c r="E3">
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H13" si="2">F3/SUM(E3:G3)</f>
+        <f>F3/SUM(E3:G3)</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -532,14 +532,14 @@
         <v>39029</v>
       </c>
       <c r="B4" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A4)</f>
         <v>11</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="1"/>
+        <f>DAY(A4)</f>
         <v>8</v>
       </c>
       <c r="E4">
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
+        <f>F4/SUM(E4:G4)</f>
         <v>0</v>
       </c>
       <c r="I4" t="s">
@@ -564,14 +564,14 @@
         <v>39030</v>
       </c>
       <c r="B5" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A5)</f>
         <v>11</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
+        <f>DAY(A5)</f>
         <v>9</v>
       </c>
       <c r="E5">
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f>F5/SUM(E5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -593,31 +593,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>40136</v>
+        <v>39049</v>
       </c>
       <c r="B6" s="2">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A6)</f>
         <v>11</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f>DAY(A6)</f>
+        <v>28</v>
       </c>
       <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>22</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>F6/SUM(E6:G6)</f>
+        <v>0.62857142857142856</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -625,63 +625,63 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43795</v>
+        <v>39054</v>
       </c>
       <c r="B7" s="2">
-        <v>2019</v>
+        <v>2007</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>MONTH(A7)</f>
+        <v>12</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f>DAY(A7)</f>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>F7/SUM(E7:G7)</f>
+        <v>0.875</v>
       </c>
       <c r="I7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>39049</v>
+        <v>39414</v>
       </c>
       <c r="B8" s="2">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A8)</f>
         <v>11</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
+        <f>DAY(A8)</f>
         <v>28</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F8">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
-        <v>0.62857142857142856</v>
+        <f>F8/SUM(E8:G8)</f>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>8</v>
@@ -689,21 +689,21 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>39414</v>
+        <v>40136</v>
       </c>
       <c r="B9" s="2">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A9)</f>
         <v>11</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f>DAY(A9)</f>
+        <v>19</v>
       </c>
       <c r="E9">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
+        <f>F9/SUM(E9:G9)</f>
         <v>0</v>
       </c>
       <c r="I9" t="s">
@@ -724,14 +724,14 @@
         <v>42705</v>
       </c>
       <c r="B10" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A10)</f>
         <v>12</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
+        <f>DAY(A10)</f>
         <v>1</v>
       </c>
       <c r="E10">
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f>F10/SUM(E10:G10)</f>
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -753,103 +753,103 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43436</v>
+        <v>42711</v>
       </c>
       <c r="B11" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A11)</f>
         <v>12</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>DAY(A11)</f>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>F11/SUM(E11:G11)</f>
+        <v>0.72499999999999998</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>39054</v>
+        <v>43436</v>
       </c>
       <c r="B12" s="2">
-        <v>2006</v>
+        <v>2019</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
+        <f>MONTH(A12)</f>
         <v>12</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>DAY(A12)</f>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>0.875</v>
+        <f>F12/SUM(E12:G12)</f>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>42711</v>
+        <v>43795</v>
       </c>
       <c r="B13" s="2">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>MONTH(A13)</f>
+        <v>11</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>DAY(A13)</f>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>0.72499999999999998</v>
+        <f>F13/SUM(E13:G13)</f>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
-    <sortCondition ref="C1:C15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
+    <sortCondition ref="B1:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>